<commit_message>
Roxima Child und Roxima Dateien
</commit_message>
<xml_diff>
--- a/Dokumente/Landingpages Inhalte die Orgas liefern muessen.xlsx
+++ b/Dokumente/Landingpages Inhalte die Orgas liefern muessen.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
   <si>
     <t>Slider</t>
   </si>
@@ -62,10 +62,6 @@
     <t>Ergänzender Untertitel</t>
   </si>
   <si>
-    <t>Folgende Texte und Bilder müssen für die Landingpage jeder Reise an Ruth geliefert werden
-Als Beispiel kann die Toskana Seite genutzt werden: https://rennrad-reise-toskana.com</t>
-  </si>
-  <si>
     <t>Widget 2</t>
   </si>
   <si>
@@ -105,9 +101,6 @@
     <t>Widget 3</t>
   </si>
   <si>
-    <t>Genau 1 Bild mit 1920x800 px</t>
-  </si>
-  <si>
     <t>Mehrere schöne Bilder</t>
   </si>
   <si>
@@ -123,9 +116,6 @@
     <t xml:space="preserve"> - Untertitel</t>
   </si>
   <si>
-    <t>Min. 4, max. 7 Bilder</t>
-  </si>
-  <si>
     <t>Widget 4</t>
   </si>
   <si>
@@ -345,9 +335,6 @@
     <t>Welche Guides sind mit? Texte hat Ruth!</t>
   </si>
   <si>
-    <t>4 Leistungspakete sind optimal.</t>
-  </si>
-  <si>
     <t>z.B. Bett im Doppelzimmer, Einzelzimmer,...</t>
   </si>
   <si>
@@ -364,13 +351,43 @@
   </si>
   <si>
     <t>Jedoch: Google mag guten Content (Text)</t>
+  </si>
+  <si>
+    <t>Genau 1 super Bild mit 1920x800 px was unter die Haut geht :-)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Folgende Texte und Bilder müssen für die Landingpage jeder Reise an Ruth geliefert werden
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>Als Beispiel kann die Toskana Seite genutzt werden: https://rennrad-reise-toskana.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Min. 5, max. 8 Bilder</t>
+  </si>
+  <si>
+    <t>Emotional ansprechend... Soll Lust auf die Reise machen</t>
+  </si>
+  <si>
+    <t>Ergänzung dazu....</t>
+  </si>
+  <si>
+    <t>3 bis 4 Leistungspakete sind optimal (Max 4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -392,6 +409,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -424,10 +447,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -707,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,25 +743,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="5"/>
+      <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -758,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -772,10 +795,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -786,7 +809,7 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -797,381 +820,387 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>110</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
         <v>64</v>
-      </c>
-      <c r="B40" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C44" s="6" t="s">
-        <v>108</v>
+      <c r="C44" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" t="s">
         <v>82</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D48" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D51" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D53" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D54" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D55" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D56" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D57" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D58" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D59" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D60" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D61" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.2">
@@ -1179,17 +1208,17 @@
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D63" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D64" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D65" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Liste für Orgas angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Landingpages Inhalte die Orgas liefern muessen.xlsx
+++ b/Dokumente/Landingpages Inhalte die Orgas liefern muessen.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>Slider</t>
   </si>
@@ -248,21 +248,6 @@
     <t>Enter the first one in Latitude and the second in Longitude.</t>
   </si>
   <si>
-    <t>Latitude und Longitude der Reise</t>
-  </si>
-  <si>
-    <t>Standortreise den Standort/Etappenreise den Start</t>
-  </si>
-  <si>
-    <t>Ort suchen</t>
-  </si>
-  <si>
-    <t>Rechtsklick an gewünschte Stelle. Auswahl: "Was ist hier?"</t>
-  </si>
-  <si>
-    <t>Die Zahlen, die nun unter dem Text erscheinen aufschreiben.</t>
-  </si>
-  <si>
     <t>SEO Text</t>
   </si>
   <si>
@@ -272,9 +257,6 @@
     <t xml:space="preserve">Ein ausführlicher Text </t>
   </si>
   <si>
-    <t>Anleitung: http://maps.google.de</t>
-  </si>
-  <si>
     <t>Der OnePager hat insgesamt wenig Text</t>
   </si>
   <si>
@@ -336,12 +318,6 @@
   </si>
   <si>
     <t>z.B. Bett im Doppelzimmer, Einzelzimmer,...</t>
-  </si>
-  <si>
-    <t>Brauchen wir für die Karte hinter dem</t>
-  </si>
-  <si>
-    <t>Kontaktformular</t>
   </si>
   <si>
     <t>Minimum 300 Wörter, Maximum ist open</t>
@@ -381,6 +357,18 @@
   </si>
   <si>
     <t>3 bis 4 Leistungspakete sind optimal (Max 4)</t>
+  </si>
+  <si>
+    <t>Zusatzinfos</t>
+  </si>
+  <si>
+    <t>Link zum Hotel</t>
+  </si>
+  <si>
+    <t>Evtl. Link zum Flughafen</t>
+  </si>
+  <si>
+    <t>Sonstige wichtige Infos oder Links</t>
   </si>
 </sst>
 </file>
@@ -730,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,7 +732,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -795,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
@@ -923,7 +911,7 @@
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
         <v>72</v>
@@ -934,7 +922,7 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -942,7 +930,7 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -953,15 +941,15 @@
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
@@ -978,7 +966,7 @@
         <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -994,7 +982,7 @@
         <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1083,124 +1071,109 @@
         <v>66</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>74</v>
+        <v>106</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>103</v>
-      </c>
       <c r="D43" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C44" s="5" t="s">
-        <v>104</v>
-      </c>
+      <c r="C44" s="5"/>
       <c r="D44" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D50" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D51" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D53" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D54" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D55" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D56" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D57" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D58" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D59" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D60" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D61" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.2">
@@ -1208,17 +1181,17 @@
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D63" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D64" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D65" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.2">

</xml_diff>